<commit_message>
14 Sep 2021 Selenium Writing to Excel
</commit_message>
<xml_diff>
--- a/src/test/resources/AutomationDemoSIte.xlsx
+++ b/src/test/resources/AutomationDemoSIte.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspaces\AugustBatchSelenium2021\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspaces\JulyAutomationSelenium2021\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{2F3D61AC-072B-42F3-A178-2A1426BC425E}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{CB673EE6-2DC7-4A72-A18E-786BA34EB5A1}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
     <workbookView windowHeight="13276" windowWidth="20715" xWindow="-98" xr2:uid="{9F696F77-14B2-4A68-A1B1-E5EA60DF3651}" yWindow="-98"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="97">
   <si>
     <t>RunMode</t>
   </si>
@@ -389,14 +389,10 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
@@ -727,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A98684-4136-4155-A927-F35C3B12F23B}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2:S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -856,7 +852,7 @@
       <c r="R2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="S2" t="s" s="15">
+      <c r="S2" t="s" s="11">
         <v>96</v>
       </c>
     </row>
@@ -864,7 +860,7 @@
       <c r="A3" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C3" t="s">
@@ -915,7 +911,7 @@
       <c r="R3" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="S3" t="s" s="16">
+      <c r="S3" t="s" s="12">
         <v>96</v>
       </c>
     </row>
@@ -923,7 +919,7 @@
       <c r="A4" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C4" t="s">
@@ -974,13 +970,13 @@
       <c r="R4" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="S4" s="5"/>
+      <c r="S4" s="3"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>92</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C5" t="s">
@@ -1031,7 +1027,7 @@
       <c r="R5" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="S5" t="s" s="17">
+      <c r="S5" t="s" s="13">
         <v>96</v>
       </c>
     </row>
@@ -1039,7 +1035,7 @@
       <c r="A6" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C6" t="s">
@@ -1090,7 +1086,7 @@
       <c r="R6" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="S6" t="s" s="18">
+      <c r="S6" t="s" s="14">
         <v>96</v>
       </c>
     </row>
@@ -1098,7 +1094,7 @@
       <c r="A7" t="s">
         <v>93</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C7" t="s">
@@ -1149,13 +1145,13 @@
       <c r="R7" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="S7" s="8"/>
+      <c r="S7" s="4"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C8" t="s">
@@ -1206,7 +1202,7 @@
       <c r="R8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="S8" t="s" s="19">
+      <c r="S8" t="s" s="15">
         <v>96</v>
       </c>
     </row>

</xml_diff>